<commit_message>
Run using final data from 11-2022 lit update
Also update forest plot and section descriptions.
</commit_message>
<xml_diff>
--- a/Sample_Timing.xlsx
+++ b/Sample_Timing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/larsen_alexandra_epa_gov/Documents/Projects/IRIS/PFAS/PFNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="876" documentId="8_{2E2A9C82-0E17-45B6-BDC7-3E14BE1F0CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C01924C-8620-447F-A34A-D5EC33C64F4E}"/>
+  <xr:revisionPtr revIDLastSave="885" documentId="8_{2E2A9C82-0E17-45B6-BDC7-3E14BE1F0CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB05C13B-789E-4BDE-AC20-F7E2AD4F2BAD}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-2376" windowWidth="23256" windowHeight="12576" xr2:uid="{05938AA7-E8C2-4C5F-827D-4F40CB103E84}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{05938AA7-E8C2-4C5F-827D-4F40CB103E84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_Timing" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,11 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Average GA at birth: 38.6 ± 2.32 weeks.</t>
+    Average GA at birth: 38.6 ± 2.32 weeks.
+Reply:
+    Average GA at sampling: 11.3 weeks
+Reply:
+    Cite email communication</t>
       </text>
     </comment>
   </commentList>
@@ -74,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="163">
   <si>
     <t>Author</t>
   </si>
@@ -563,9 +567,6 @@
   </si>
   <si>
     <t>Chang</t>
-  </si>
-  <si>
-    <t>Chang, 2022</t>
   </si>
 </sst>
 </file>
@@ -1036,6 +1037,12 @@
   <threadedComment ref="A30" dT="2022-11-28T20:08:31.61" personId="{5BC90ED0-34B2-42AB-845D-7EE4E23BC744}" id="{3220DE42-779E-4304-8A92-E90C4A35E877}">
     <text>Average GA at birth: 38.6 ± 2.32 weeks.</text>
   </threadedComment>
+  <threadedComment ref="A30" dT="2022-11-30T15:01:11.26" personId="{5BC90ED0-34B2-42AB-845D-7EE4E23BC744}" id="{33ED33F7-B1DB-426E-92B5-61E154B50BA9}" parentId="{3220DE42-779E-4304-8A92-E90C4A35E877}">
+    <text>Average GA at sampling: 11.3 weeks</text>
+  </threadedComment>
+  <threadedComment ref="A30" dT="2022-11-30T15:01:33.25" personId="{5BC90ED0-34B2-42AB-845D-7EE4E23BC744}" id="{CE892EBB-0FC1-4CC9-A2F8-A0AC2D6BCC6E}" parentId="{3220DE42-779E-4304-8A92-E90C4A35E877}">
+    <text>Cite email communication</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1043,9 +1050,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF30337A-51E4-4717-B453-026523922710}">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2455,15 +2462,20 @@
       <c r="C30" t="s">
         <v>4</v>
       </c>
-      <c r="F30">
-        <f>Supplemental_Calculations!C103</f>
-        <v>11</v>
+      <c r="E30">
+        <v>11.4</v>
       </c>
       <c r="J30">
-        <v>8</v>
+        <v>8.1</v>
+      </c>
+      <c r="K30">
+        <v>9.6</v>
+      </c>
+      <c r="L30">
+        <v>12.6</v>
       </c>
       <c r="M30">
-        <v>14</v>
+        <v>14.6</v>
       </c>
       <c r="N30">
         <v>0</v>
@@ -2505,10 +2517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0297CC93-5BAF-45F8-8120-ADD14EA6E813}">
-  <dimension ref="B2:J103"/>
+  <dimension ref="B2:J100"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:XFD98"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99:H103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3192,45 +3204,14 @@
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B99" s="13" t="s">
-        <v>163</v>
-      </c>
+      <c r="B99" s="13"/>
       <c r="C99" s="13"/>
       <c r="D99" s="13"/>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B100" s="12" t="s">
-        <v>49</v>
-      </c>
+      <c r="B100" s="12"/>
       <c r="C100" s="12"/>
       <c r="D100" s="12"/>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B101" t="s">
-        <v>130</v>
-      </c>
-      <c r="C101">
-        <f>Sample_Timing!M30</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B102" t="s">
-        <v>129</v>
-      </c>
-      <c r="C102">
-        <f>Sample_Timing!J30</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B103" t="s">
-        <v>132</v>
-      </c>
-      <c r="C103">
-        <f>SUM(C101, C102)/2</f>
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="26">

</xml_diff>

<commit_message>
Add analysis for early vs late sampling within high confidence studies only
</commit_message>
<xml_diff>
--- a/Sample_Timing.xlsx
+++ b/Sample_Timing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/larsen_alexandra_epa_gov/Documents/Projects/IRIS/PFAS/PFNA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/larsen_alexandra_epa_gov/Documents/Projects/IRIS/PFAS/pfas-birthweight-meta-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="885" documentId="8_{2E2A9C82-0E17-45B6-BDC7-3E14BE1F0CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB05C13B-789E-4BDE-AC20-F7E2AD4F2BAD}"/>
+  <xr:revisionPtr revIDLastSave="886" documentId="8_{2E2A9C82-0E17-45B6-BDC7-3E14BE1F0CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{880F9CF9-9824-40A9-A0BF-E288382583EB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{05938AA7-E8C2-4C5F-827D-4F40CB103E84}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{05938AA7-E8C2-4C5F-827D-4F40CB103E84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_Timing" sheetId="1" r:id="rId1"/>
@@ -170,9 +170,6 @@
     <t>Valvi</t>
   </si>
   <si>
-    <t>Wikström</t>
-  </si>
-  <si>
     <t>Ashley-Martin</t>
   </si>
   <si>
@@ -567,6 +564,9 @@
   </si>
   <si>
     <t>Chang</t>
+  </si>
+  <si>
+    <t>Wikstrom</t>
   </si>
 </sst>
 </file>
@@ -682,10 +682,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -694,16 +694,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -1050,22 +1050,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF30337A-51E4-4717-B453-026523922710}">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
@@ -1127,16 +1127,16 @@
         <v>14</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="T6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U6" t="s">
         <v>28</v>
@@ -1377,7 +1377,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1421,9 +1421,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>162</v>
       </c>
       <c r="B8">
         <v>2020</v>
@@ -1465,9 +1465,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9">
         <v>2017</v>
@@ -1510,9 +1510,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>2016</v>
@@ -1561,9 +1561,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B11">
         <v>2018</v>
@@ -1612,15 +1612,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12">
         <v>2016</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <f>Supplemental_Calculations!C29</f>
@@ -1657,9 +1657,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B13">
         <v>2018</v>
@@ -1699,12 +1699,12 @@
         <v>28</v>
       </c>
       <c r="W13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14">
         <v>2010</v>
@@ -1753,9 +1753,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15">
         <v>2016</v>
@@ -1786,21 +1786,21 @@
         <v>0</v>
       </c>
       <c r="T15" t="s">
+        <v>85</v>
+      </c>
+      <c r="U15" t="s">
+        <v>28</v>
+      </c>
+      <c r="V15" t="s">
+        <v>28</v>
+      </c>
+      <c r="W15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>86</v>
-      </c>
-      <c r="U15" t="s">
-        <v>28</v>
-      </c>
-      <c r="V15" t="s">
-        <v>28</v>
-      </c>
-      <c r="W15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>87</v>
       </c>
       <c r="B16">
         <v>2018</v>
@@ -1837,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="T16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U16" t="s">
         <v>28</v>
@@ -1849,15 +1849,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17">
         <v>2016</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H17">
         <v>40</v>
@@ -1890,18 +1890,18 @@
         <v>28</v>
       </c>
       <c r="W17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B18">
         <v>2017</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D18">
         <v>39</v>
@@ -1934,18 +1934,18 @@
         <v>28</v>
       </c>
       <c r="W18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B19">
         <v>2017</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19">
         <f>Supplemental_Calculations!C70</f>
@@ -1983,18 +1983,18 @@
         <v>28</v>
       </c>
       <c r="W19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B20">
         <v>2019</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20">
         <f>Supplemental_Calculations!C78</f>
@@ -2032,12 +2032,12 @@
         <v>28</v>
       </c>
       <c r="W20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B21">
         <v>2015</v>
@@ -2079,9 +2079,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B22">
         <v>2016</v>
@@ -2124,15 +2124,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B23">
         <v>2012</v>
       </c>
       <c r="C23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E23">
         <v>39</v>
@@ -2165,12 +2165,12 @@
         <v>28</v>
       </c>
       <c r="W23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24">
         <v>2020</v>
@@ -2212,9 +2212,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B25">
         <v>2020</v>
@@ -2263,9 +2263,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B26">
         <v>2021</v>
@@ -2313,9 +2313,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B27">
         <v>2021</v>
@@ -2357,9 +2357,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B28" s="10">
         <v>2019</v>
@@ -2396,7 +2396,7 @@
         <v>0</v>
       </c>
       <c r="T28" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U28" s="10" t="s">
         <v>28</v>
@@ -2408,9 +2408,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B29">
         <v>2021</v>
@@ -2452,9 +2452,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B30">
         <v>2022</v>
@@ -2519,19 +2519,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0297CC93-5BAF-45F8-8120-ADD14EA6E813}">
   <dimension ref="B2:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="A99" sqref="A99:H103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -2539,9 +2539,9 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="12" t="s">
-        <v>36</v>
+    <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -2549,552 +2549,552 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>13.8</v>
       </c>
       <c r="E6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <f>SUM(C5, C6)/2</f>
         <v>9.9</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>39</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>40</v>
       </c>
       <c r="C12">
         <f>Sample_Timing!J10</f>
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13">
         <v>13.8</v>
       </c>
       <c r="E13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15">
         <f>Sample_Timing!M10</f>
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16">
         <v>0.96</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17">
         <f>C16*((C12+C13)/2)+(1-C16)*((C14+C15)/2)</f>
         <v>11.623999999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="13" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21">
         <f>Sample_Timing!J11</f>
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <f>Sample_Timing!M11</f>
         <v>13.9</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23">
         <f>(C21+C22)/2</f>
         <v>11.95</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="13" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28">
         <v>39.700000000000003</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29">
         <f>C28-2</f>
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="13" t="s">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B32" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34">
         <f>280/7</f>
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35">
         <f>C34+3</f>
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40">
         <f>Sample_Timing!J14</f>
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C41">
         <f>Sample_Timing!M14</f>
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C42">
         <f>(C40+C41)/2</f>
         <v>15.5</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="13" t="s">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="12" t="s">
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>81</v>
-      </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>82</v>
       </c>
       <c r="C47">
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C49">
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C50">
         <v>0.18</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C51">
         <v>0.32</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C52">
         <v>0.49</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C53">
         <f>C50*C47+C51*C48+C52*C49</f>
         <v>25.21</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B55" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B56" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C58">
         <f>Sample_Timing!J16</f>
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C59">
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C60">
         <f>Sample_Timing!M16</f>
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C61">
         <v>0.86</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C62">
         <v>0.09</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C63">
         <v>0.05</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C64">
         <f>C61*C58+C62*C59+C63*C60</f>
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B66" s="13" t="s">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B67" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C69">
         <v>275.5</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C70">
         <f>C69/7</f>
         <v>39.357142857142854</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C71">
         <v>29.6</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C72">
         <f>C71/7</f>
         <v>4.2285714285714286</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B74" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B75" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C77">
         <v>275.7</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C78">
         <f>C77/7</f>
         <v>39.385714285714286</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C79">
         <v>9.6</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C80">
         <f>C79/7</f>
         <v>1.3714285714285714</v>
       </c>
     </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B82" s="13" t="s">
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B82" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B83" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C82" s="13"/>
-      <c r="D82" s="13"/>
-    </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B83" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C83" s="12"/>
-      <c r="D83" s="12"/>
-    </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C85">
         <v>39</v>
       </c>
       <c r="D85" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C86">
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C87">
         <f>(C85+C86)/2</f>
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B89" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="C89" s="13"/>
-      <c r="D89" s="13"/>
+    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B89" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
     </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B90" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
-    </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B90" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C92" s="4">
         <f>Sample_Timing!J25</f>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="D92" s="4"/>
       <c r="E92" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F92">
         <v>1</v>
@@ -3120,9 +3120,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C93" s="4">
         <f>Sample_Timing!M25</f>
@@ -3130,7 +3130,7 @@
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F93">
         <v>2010</v>
@@ -3148,16 +3148,16 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C94">
         <v>7</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F94">
         <v>57</v>
@@ -3175,18 +3175,18 @@
         <v>76</v>
       </c>
     </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C95">
         <v>13.8</v>
       </c>
       <c r="E95" s="4"/>
     </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B96" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C96" s="4">
         <f>SUM(F94:G94)/SUM(F94:J94)</f>
@@ -3194,37 +3194,27 @@
       </c>
       <c r="F96" s="4"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C97">
         <f>C96*((C92+C93)/2)+(1-C96)*((C94+C95)/2)</f>
         <v>15.387866108786612</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B99" s="13"/>
-      <c r="C99" s="13"/>
-      <c r="D99" s="13"/>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B100" s="12"/>
-      <c r="C100" s="12"/>
-      <c r="D100" s="12"/>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="12"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="12"/>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="13"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="B100:D100"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B75:D75"/>
     <mergeCell ref="B45:D45"/>
     <mergeCell ref="B55:D55"/>
     <mergeCell ref="B56:D56"/>
@@ -3241,6 +3231,16 @@
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B75:D75"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3256,23 +3256,23 @@
       <selection activeCell="D19" sqref="D19:O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>113</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>114</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
@@ -3286,556 +3286,565 @@
       <c r="N1" s="19"/>
       <c r="O1" s="19"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="B4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="D4" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="16" t="s">
+      <c r="B5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="D5" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="18" t="s">
+      <c r="B11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
-      <c r="B13" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
-      <c r="B14" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="B16" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="21"/>
-      <c r="B18" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="17" t="s">
+      <c r="B22" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="17" t="s">
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="20" t="s">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="17" t="s">
+      <c r="C24" s="17"/>
+      <c r="D24" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
-      <c r="B24" s="20" t="s">
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="17" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
-      <c r="B25" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D21:O21"/>
-    <mergeCell ref="D22:O22"/>
-    <mergeCell ref="D23:O23"/>
-    <mergeCell ref="D24:O24"/>
-    <mergeCell ref="D25:O25"/>
+    <mergeCell ref="D2:O2"/>
+    <mergeCell ref="D13:O13"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D8:O8"/>
+    <mergeCell ref="D9:O9"/>
+    <mergeCell ref="D10:O10"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:O11"/>
+    <mergeCell ref="D12:O12"/>
+    <mergeCell ref="D7:O7"/>
+    <mergeCell ref="D6:O6"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D5:O5"/>
+    <mergeCell ref="D4:O4"/>
+    <mergeCell ref="D3:O3"/>
     <mergeCell ref="D20:O20"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -3852,30 +3861,21 @@
     <mergeCell ref="D17:O17"/>
     <mergeCell ref="D18:O18"/>
     <mergeCell ref="D19:O19"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:O1"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:O11"/>
-    <mergeCell ref="D12:O12"/>
-    <mergeCell ref="D7:O7"/>
-    <mergeCell ref="D6:O6"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D5:O5"/>
-    <mergeCell ref="D4:O4"/>
-    <mergeCell ref="D3:O3"/>
-    <mergeCell ref="D2:O2"/>
-    <mergeCell ref="D13:O13"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D8:O8"/>
-    <mergeCell ref="D9:O9"/>
-    <mergeCell ref="D10:O10"/>
+    <mergeCell ref="D21:O21"/>
+    <mergeCell ref="D22:O22"/>
+    <mergeCell ref="D23:O23"/>
+    <mergeCell ref="D24:O24"/>
+    <mergeCell ref="D25:O25"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding data for PFOS
new spreadsheet
</commit_message>
<xml_diff>
--- a/Sample_Timing.xlsx
+++ b/Sample_Timing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/larsen_alexandra_epa_gov/Documents/Projects/IRIS/PFAS/pfas-birthweight-meta-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="886" documentId="8_{2E2A9C82-0E17-45B6-BDC7-3E14BE1F0CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{880F9CF9-9824-40A9-A0BF-E288382583EB}"/>
+  <xr:revisionPtr revIDLastSave="914" documentId="8_{2E2A9C82-0E17-45B6-BDC7-3E14BE1F0CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8298B9D4-8FF2-4832-BF8E-B5AFFBDCE253}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{05938AA7-E8C2-4C5F-827D-4F40CB103E84}"/>
+    <workbookView xWindow="285" yWindow="1290" windowWidth="26715" windowHeight="13200" xr2:uid="{05938AA7-E8C2-4C5F-827D-4F40CB103E84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_Timing" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="166">
   <si>
     <t>Author</t>
   </si>
@@ -567,6 +567,15 @@
   </si>
   <si>
     <t>Wikstrom</t>
+  </si>
+  <si>
+    <t>PFNA</t>
+  </si>
+  <si>
+    <t>PFHxS</t>
+  </si>
+  <si>
+    <t>PFOS</t>
   </si>
 </sst>
 </file>
@@ -682,10 +691,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -694,16 +703,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -1048,11 +1057,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF30337A-51E4-4717-B453-026523922710}">
-  <dimension ref="A1:W30"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,7 +1074,7 @@
     <col min="8" max="8" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1135,8 +1144,17 @@
       <c r="W1" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1185,8 +1203,11 @@
       <c r="W2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1232,8 +1253,11 @@
       <c r="W3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1276,8 +1300,11 @@
       <c r="W4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1326,8 +1353,11 @@
       <c r="W5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1376,8 +1406,11 @@
       <c r="W6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1420,8 +1453,11 @@
       <c r="W7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -1464,8 +1500,11 @@
       <c r="W8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1509,8 +1548,11 @@
       <c r="W9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1560,8 +1602,11 @@
       <c r="W10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>146</v>
       </c>
@@ -1611,8 +1656,11 @@
       <c r="W11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1656,8 +1704,11 @@
       <c r="W12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>147</v>
       </c>
@@ -1701,8 +1752,11 @@
       <c r="W13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -1752,8 +1806,11 @@
       <c r="W14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -1797,8 +1854,11 @@
       <c r="W15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -1848,8 +1908,11 @@
       <c r="W16" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -1892,8 +1955,11 @@
       <c r="W17" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>114</v>
       </c>
@@ -1936,8 +2002,11 @@
       <c r="W18" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>115</v>
       </c>
@@ -1985,8 +2054,11 @@
       <c r="W19" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>122</v>
       </c>
@@ -2034,8 +2106,11 @@
       <c r="W20" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -2079,7 +2154,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>125</v>
       </c>
@@ -2124,7 +2199,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>132</v>
       </c>
@@ -2168,7 +2243,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>134</v>
       </c>
@@ -2212,7 +2287,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>135</v>
       </c>
@@ -2263,7 +2338,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>132</v>
       </c>
@@ -2312,8 +2387,11 @@
       <c r="W26" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>154</v>
       </c>
@@ -2356,8 +2434,11 @@
       <c r="W27" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>155</v>
       </c>
@@ -2407,8 +2488,11 @@
       <c r="W28" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y28" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>160</v>
       </c>
@@ -2451,8 +2535,11 @@
       <c r="W29" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>161</v>
       </c>
@@ -2506,6 +2593,9 @@
       </c>
       <c r="W30" t="s">
         <v>21</v>
+      </c>
+      <c r="Y30" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2540,7 +2630,7 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="15"/>
@@ -2581,18 +2671,18 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -2649,18 +2739,18 @@
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -2690,18 +2780,18 @@
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
@@ -2721,18 +2811,18 @@
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
@@ -2753,18 +2843,18 @@
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
@@ -2794,18 +2884,18 @@
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
@@ -2865,18 +2955,18 @@
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
@@ -2938,18 +3028,18 @@
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="12" t="s">
+      <c r="B66" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
@@ -2986,18 +3076,18 @@
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="12" t="s">
+      <c r="B74" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="13" t="s">
+      <c r="B75" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
@@ -3034,18 +3124,18 @@
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B82" s="12" t="s">
+      <c r="B82" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B83" s="13" t="s">
+      <c r="B83" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
@@ -3076,21 +3166,21 @@
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B89" s="12" t="s">
+      <c r="B89" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B90" s="13" t="s">
+      <c r="B90" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
@@ -3204,17 +3294,27 @@
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="12"/>
-      <c r="C99" s="12"/>
-      <c r="D99" s="12"/>
+      <c r="B99" s="13"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="13"/>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
-      <c r="D100" s="13"/>
+      <c r="B100" s="12"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B75:D75"/>
     <mergeCell ref="B45:D45"/>
     <mergeCell ref="B55:D55"/>
     <mergeCell ref="B56:D56"/>
@@ -3231,16 +3331,6 @@
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="B100:D100"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B75:D75"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3287,548 +3377,571 @@
       <c r="O1" s="19"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21" t="s">
+      <c r="B2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="21" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="20" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="20" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="20" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="20" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="18" t="s">
+      <c r="C10" s="18"/>
+      <c r="D10" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17" t="s">
+      <c r="A13" s="21"/>
+      <c r="B13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18" t="s">
+      <c r="C13" s="20"/>
+      <c r="D13" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18" t="s">
+      <c r="C14" s="20"/>
+      <c r="D14" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17" t="s">
+      <c r="A18" s="21"/>
+      <c r="B18" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17" t="s">
+      <c r="A19" s="21"/>
+      <c r="B19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18" t="s">
+      <c r="C19" s="20"/>
+      <c r="D19" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17" t="s">
+      <c r="A20" s="21"/>
+      <c r="B20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18" t="s">
+      <c r="C20" s="20"/>
+      <c r="D20" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17" t="s">
+      <c r="A21" s="21"/>
+      <c r="B21" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18" t="s">
+      <c r="C21" s="20"/>
+      <c r="D21" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18" t="s">
+      <c r="C22" s="20"/>
+      <c r="D22" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17" t="s">
+      <c r="A23" s="21"/>
+      <c r="B23" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18" t="s">
+      <c r="C23" s="20"/>
+      <c r="D23" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17" t="s">
+      <c r="A24" s="21"/>
+      <c r="B24" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="18" t="s">
+      <c r="C24" s="20"/>
+      <c r="D24" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17" t="s">
+      <c r="A25" s="21"/>
+      <c r="B25" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="18" t="s">
+      <c r="C25" s="20"/>
+      <c r="D25" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="D2:O2"/>
-    <mergeCell ref="D13:O13"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D8:O8"/>
-    <mergeCell ref="D9:O9"/>
-    <mergeCell ref="D10:O10"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D21:O21"/>
+    <mergeCell ref="D22:O22"/>
+    <mergeCell ref="D23:O23"/>
+    <mergeCell ref="D24:O24"/>
+    <mergeCell ref="D25:O25"/>
+    <mergeCell ref="D20:O20"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D14:O14"/>
+    <mergeCell ref="D15:O15"/>
+    <mergeCell ref="D16:O16"/>
+    <mergeCell ref="D17:O17"/>
+    <mergeCell ref="D18:O18"/>
+    <mergeCell ref="D19:O19"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:O1"/>
     <mergeCell ref="B11:C11"/>
@@ -3845,37 +3958,14 @@
     <mergeCell ref="D5:O5"/>
     <mergeCell ref="D4:O4"/>
     <mergeCell ref="D3:O3"/>
-    <mergeCell ref="D20:O20"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D14:O14"/>
-    <mergeCell ref="D15:O15"/>
-    <mergeCell ref="D16:O16"/>
-    <mergeCell ref="D17:O17"/>
-    <mergeCell ref="D18:O18"/>
-    <mergeCell ref="D19:O19"/>
-    <mergeCell ref="D21:O21"/>
-    <mergeCell ref="D22:O22"/>
-    <mergeCell ref="D23:O23"/>
-    <mergeCell ref="D24:O24"/>
-    <mergeCell ref="D25:O25"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="D2:O2"/>
+    <mergeCell ref="D13:O13"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D8:O8"/>
+    <mergeCell ref="D9:O9"/>
+    <mergeCell ref="D10:O10"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>